<commit_message>
study font size and participant update
</commit_message>
<xml_diff>
--- a/study_distractor/participant.xlsx
+++ b/study_distractor/participant.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6760" yWindow="7160" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="2540" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,6 @@
     <t>block 1</t>
   </si>
   <si>
-    <t>sit</t>
-  </si>
-  <si>
     <t>no distract</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>stand</t>
   </si>
 </sst>
 </file>
@@ -382,17 +382,17 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -429,20 +429,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
+    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
         <v>3</v>
       </c>
     </row>
@@ -497,20 +497,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
         <v>3</v>
       </c>
     </row>
@@ -565,20 +565,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>4</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
         <v>3</v>
       </c>
     </row>
@@ -633,20 +633,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
         <v>3</v>
       </c>
     </row>
@@ -672,43 +672,43 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" t="s">
-        <v>6</v>
-      </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>